<commit_message>
Getting closer to understanding Alt2
</commit_message>
<xml_diff>
--- a/Excel_Challenge_596 - Increment Sequences.xlsx
+++ b/Excel_Challenge_596 - Increment Sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B89F19-9BA9-498C-BE51-12BFDD9AFEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C749844D-2278-4887-9812-E7CE1B873BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -605,7 +605,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="748" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45BAD9-77AA-4B9B-9B91-E0B0D9F56C3A}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1248,89 +1248,297 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" cm="1">
         <f t="array" ref="B22:B38">_xlfn.LET(_xlpm.a,A2:A18,_xlpm.b,_xlfn.SCAN(0,_xlfn.DROP(_xlfn.VSTACK(0,_xlpm.a),-1)&lt;&gt;_xlpm.a,_xleta.SUM),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,(_xlpm.c&gt;0)*_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D22" t="str" cm="1">
+        <f t="array" ref="D22:D38">A2:A18</f>
+        <v>A</v>
+      </c>
+      <c r="E22" cm="1">
+        <f t="array" ref="E22:E38">_xlfn.SCAN(0,_xlfn.DROP(_xlfn.VSTACK(0,_xlfn.ANCHORARRAY(D22)),-1)&lt;&gt;_xlfn.ANCHORARRAY(D22),_xleta.SUM)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22:F38">_xlfn.LET(_xlpm.a,_xlfn.ANCHORARRAY(D22),_xlpm.b,_xlfn.ANCHORARRAY(E22),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,(_xlpm.c&gt;0)*_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
+        <v>1</v>
+      </c>
+      <c r="G22" cm="1">
+        <f t="array" ref="G22:G38">_xlfn.LET(_xlpm.a,_xlfn.ANCHORARRAY(D22),_xlpm.b,_xlfn.ANCHORARRAY(E22),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D23" t="str">
+        <v>A</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D24" t="str">
+        <v>A</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D27" t="str">
+        <v>B</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D29" t="str">
+        <v>C</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D30" t="str">
+        <v>C</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D32" t="str">
+        <v>C</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D33" t="str">
+        <v>C</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D34" t="str">
+        <v>C</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D35" t="str">
+        <v>B</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="D37" t="str">
+        <v>B</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="D38" t="str">
+        <v>A</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I think I now understand it
</commit_message>
<xml_diff>
--- a/Excel_Challenge_596 - Increment Sequences.xlsx
+++ b/Excel_Challenge_596 - Increment Sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C749844D-2278-4887-9812-E7CE1B873BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA079ED-B2ED-414C-B6AE-5FF7343F94EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22:E38"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22" cm="1">
         <f t="array" ref="B22:B38">_xlfn.LET(_xlpm.a,A2:A18,_xlpm.b,_xlfn.SCAN(0,_xlfn.DROP(_xlfn.VSTACK(0,_xlpm.a),-1)&lt;&gt;_xlpm.a,_xleta.SUM),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,(_xlpm.c&gt;0)*_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
         <v>1</v>
@@ -1269,8 +1269,12 @@
         <f t="array" ref="G22:G38">_xlfn.LET(_xlpm.a,_xlfn.ANCHORARRAY(D22),_xlpm.b,_xlfn.ANCHORARRAY(E22),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I22" cm="1">
+        <f t="array" ref="I22:I23">_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(E22),_xlfn.ANCHORARRAY(D22)="A"))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1</v>
       </c>
@@ -1286,8 +1290,11 @@
       <c r="G23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1304,7 +1311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0</v>
       </c>
@@ -1321,7 +1328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0</v>
       </c>
@@ -1338,7 +1345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>1</v>
       </c>
@@ -1355,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>1</v>
       </c>
@@ -1389,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1406,7 +1413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1423,7 +1430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
I have duplicated using separate functions
</commit_message>
<xml_diff>
--- a/Excel_Challenge_596 - Increment Sequences.xlsx
+++ b/Excel_Challenge_596 - Increment Sequences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA079ED-B2ED-414C-B6AE-5FF7343F94EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD4B63-9671-455D-9DFA-2088902C0020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="6">
   <si>
     <t>Alphabets</t>
   </si>
@@ -605,7 +605,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="511" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45BAD9-77AA-4B9B-9B91-E0B0D9F56C3A}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1248,7 +1248,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B22" cm="1">
         <f t="array" ref="B22:B38">_xlfn.LET(_xlpm.a,A2:A18,_xlpm.b,_xlfn.SCAN(0,_xlfn.DROP(_xlfn.VSTACK(0,_xlpm.a),-1)&lt;&gt;_xlpm.a,_xleta.SUM),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,(_xlpm.c&gt;0)*_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
         <v>1</v>
@@ -1273,8 +1278,23 @@
         <f t="array" ref="I22:I23">_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(E22),_xlfn.ANCHORARRAY(D22)="A"))</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K22" cm="1">
+        <f t="array" ref="K22:K38">_xlfn.DROP(_xlfn.VSTACK(0,_xlfn.ANCHORARRAY(D22)),-1)</f>
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>2</v>
+      </c>
+      <c r="M22" t="b">
+        <f>K22&lt;&gt;L22</f>
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <f>M22+N21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>1</v>
       </c>
@@ -1293,8 +1313,22 @@
       <c r="I23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K23" t="str">
+        <v>A</v>
+      </c>
+      <c r="L23" t="s">
+        <v>2</v>
+      </c>
+      <c r="M23" t="b">
+        <f t="shared" ref="M23:M38" si="0">K23&lt;&gt;L23</f>
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ref="N23:N38" si="1">M23+N22</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>1</v>
       </c>
@@ -1310,8 +1344,22 @@
       <c r="G24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K24" t="str">
+        <v>A</v>
+      </c>
+      <c r="L24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>0</v>
       </c>
@@ -1327,8 +1375,22 @@
       <c r="G25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K25" t="str">
+        <v>A</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>0</v>
       </c>
@@ -1344,8 +1406,22 @@
       <c r="G26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>1</v>
       </c>
@@ -1361,8 +1437,22 @@
       <c r="G27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>3</v>
+      </c>
+      <c r="M27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>0</v>
       </c>
@@ -1378,8 +1468,22 @@
       <c r="G28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K28" t="str">
+        <v>B</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>1</v>
       </c>
@@ -1395,8 +1499,22 @@
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M29" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1412,8 +1530,22 @@
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K30" t="str">
+        <v>C</v>
+      </c>
+      <c r="L30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N30">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>0</v>
       </c>
@@ -1429,8 +1561,22 @@
       <c r="G31">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K31" t="str">
+        <v>C</v>
+      </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>2</v>
       </c>
@@ -1446,8 +1592,22 @@
       <c r="G32">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>2</v>
       </c>
@@ -1463,8 +1623,22 @@
       <c r="G33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K33" t="str">
+        <v>C</v>
+      </c>
+      <c r="L33" t="s">
+        <v>4</v>
+      </c>
+      <c r="M33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N33">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>2</v>
       </c>
@@ -1480,8 +1654,22 @@
       <c r="G34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K34" t="str">
+        <v>C</v>
+      </c>
+      <c r="L34" t="s">
+        <v>4</v>
+      </c>
+      <c r="M34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N34">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>2</v>
       </c>
@@ -1497,8 +1685,22 @@
       <c r="G35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K35" t="str">
+        <v>C</v>
+      </c>
+      <c r="L35" t="s">
+        <v>3</v>
+      </c>
+      <c r="M35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36">
         <v>0</v>
       </c>
@@ -1514,8 +1716,22 @@
       <c r="G36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K36" t="str">
+        <v>B</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37">
         <v>3</v>
       </c>
@@ -1531,8 +1747,22 @@
       <c r="G37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37" t="s">
+        <v>3</v>
+      </c>
+      <c r="M37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38">
         <v>2</v>
       </c>
@@ -1548,8 +1778,23 @@
       <c r="G38">
         <v>2</v>
       </c>
+      <c r="K38" t="str">
+        <v>B</v>
+      </c>
+      <c r="L38" t="s">
+        <v>2</v>
+      </c>
+      <c r="M38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="N38">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I am working on refining my abilities here
</commit_message>
<xml_diff>
--- a/Excel_Challenge_596 - Increment Sequences.xlsx
+++ b/Excel_Challenge_596 - Increment Sequences.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CD4B63-9671-455D-9DFA-2088902C0020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1AA0B7-C0A5-40DB-881D-5C9376FB1A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="Alt1" sheetId="2" r:id="rId2"/>
     <sheet name="Alt2" sheetId="3" r:id="rId3"/>
+    <sheet name="EDA" sheetId="5" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -60,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="6">
   <si>
     <t>Alphabets</t>
   </si>
@@ -84,7 +88,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,8 +104,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -120,6 +139,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -130,17 +155,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Intro_Hd" xfId="2" xr:uid="{C1DADFBD-4337-4DC6-A8DB-AD070D043920}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{289BC076-2E23-4435-8217-A9E275C67AC4}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -621,6 +651,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -1106,8 +1139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45BAD9-77AA-4B9B-9B91-E0B0D9F56C3A}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1797,4 +1830,330 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3E234F-01B3-488D-A5E3-B2B3F7D18E05}">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="4" cm="1">
+        <f t="array" ref="E22:E38">_xlfn.SCAN(0,_xlfn.DROP(_xlfn.VSTACK(0,D22:D38),-1)&lt;&gt;D22:D38,_xleta.SUM)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" cm="1">
+        <f t="array" ref="F22:F38">_xlfn.LET(_xlpm.a,D22:D38,_xlpm.b,_xlfn.ANCHORARRAY(E22),_xlfn.MAP(_xlpm.a,_xlpm.b,_xlfn.LAMBDA(_xlpm.c,_xlpm.d,_xlfn.XMATCH(_xlpm.d,_xlfn.UNIQUE(_xlfn._xlws.FILTER(_xlpm.b,_xlpm.a=_xlpm.c))))))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33">
+        <v>7</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>